<commit_message>
trying to find name
</commit_message>
<xml_diff>
--- a/shinyapp/data/absencerate.xlsx
+++ b/shinyapp/data/absencerate.xlsx
@@ -1,21 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandaljuba/Downloads/DSPG-R-Training/2022_DSPG_Loudoun/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandaljuba/Downloads/DSPG-R-Training/2022_DSPG_Loudoun/shinyapp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70A7BCB6-4CEF-2D40-A9D8-26FCBAAC1F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{73547709-FE69-264E-B961-CD6666D9E8E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="25140" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -40,7 +52,7 @@
     <t>Elementary School</t>
   </si>
   <si>
-    <t>Forest Grove ES</t>
+    <t xml:space="preserve">Forest Grove  </t>
   </si>
   <si>
     <t>Q1</t>
@@ -55,19 +67,19 @@
     <t>Q4</t>
   </si>
   <si>
-    <t>Guilford ES</t>
-  </si>
-  <si>
-    <t>Rolling Ridge ES</t>
-  </si>
-  <si>
-    <t>Sterling ES</t>
-  </si>
-  <si>
-    <t>Sugarland ES</t>
-  </si>
-  <si>
-    <t>Sully ES</t>
+    <t xml:space="preserve">Guilford  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rolling Ridge  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sterling  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sugarland  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sully  </t>
   </si>
 </sst>
 </file>
@@ -77,7 +89,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,15 +461,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="5" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="5" width="15.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,7 +488,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -485,13 +499,13 @@
         <v>7</v>
       </c>
       <c r="D2" s="1">
-        <v>4.0662420382165609E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="E2" s="1">
         <v>1.27898089171975E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -502,13 +516,13 @@
         <v>8</v>
       </c>
       <c r="D3" s="1">
-        <v>4.4275621794251367E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="E3" s="1">
         <v>1.3645601471015231E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -519,13 +533,13 @@
         <v>9</v>
       </c>
       <c r="D4" s="1">
-        <v>5.2436440677966163E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="E4" s="1">
         <v>1.7037429378531029E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -536,13 +550,13 @@
         <v>10</v>
       </c>
       <c r="D5" s="1">
-        <v>5.9940316937641458E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="E5" s="1">
         <v>1.399464910475412E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -553,13 +567,13 @@
         <v>7</v>
       </c>
       <c r="D6" s="1">
-        <v>6.0812052177108167E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="E6" s="1">
         <v>1.754547124747385E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -570,13 +584,13 @@
         <v>8</v>
       </c>
       <c r="D7" s="1">
-        <v>6.7835798106705036E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="E7" s="1">
         <v>2.0896043275313029E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -587,13 +601,13 @@
         <v>9</v>
       </c>
       <c r="D8" s="1">
-        <v>5.6848270881810103E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="E8" s="1">
         <v>4.0921126534542267E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -604,13 +618,13 @@
         <v>10</v>
       </c>
       <c r="D9" s="1">
-        <v>5.8366877515813709E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="E9" s="1">
         <v>3.5269311865056552E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -621,13 +635,13 @@
         <v>7</v>
       </c>
       <c r="D10" s="1">
-        <v>5.3623000991422032E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="E10" s="1">
         <v>4.0734514418724999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -638,13 +652,13 @@
         <v>8</v>
       </c>
       <c r="D11" s="1">
-        <v>6.9810773880998767E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="E11" s="1">
         <v>3.5443666928905659E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -655,13 +669,13 @@
         <v>9</v>
       </c>
       <c r="D12" s="1">
-        <v>6.654917436113561E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="E12" s="1">
         <v>3.2680740201524887E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -672,13 +686,13 @@
         <v>10</v>
       </c>
       <c r="D13" s="1">
-        <v>7.1508172362555689E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="E13" s="1">
         <v>3.4175334323922717E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -689,13 +703,13 @@
         <v>7</v>
       </c>
       <c r="D14" s="1">
-        <v>4.550953395932944E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="E14" s="1">
         <v>3.179906676651878E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -706,13 +720,13 @@
         <v>8</v>
       </c>
       <c r="D15" s="1">
-        <v>4.899839076632817E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="E15" s="1">
         <v>3.4071361189723093E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -723,13 +737,13 @@
         <v>9</v>
       </c>
       <c r="D16" s="1">
-        <v>5.0837873959083013E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="E16" s="1">
         <v>4.4515266783180851E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -740,13 +754,13 @@
         <v>10</v>
       </c>
       <c r="D17" s="1">
-        <v>5.3356176956495083E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="E17" s="1">
         <v>4.6625466560606947E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -757,13 +771,13 @@
         <v>7</v>
       </c>
       <c r="D18" s="1">
-        <v>6.5131097879452593E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="E18" s="1">
         <v>2.1988927191058161E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -774,13 +788,13 @@
         <v>8</v>
       </c>
       <c r="D19" s="1">
-        <v>7.8414053682712592E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="E19" s="1">
         <v>3.5526767751116288E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -791,13 +805,13 @@
         <v>9</v>
       </c>
       <c r="D20" s="1">
-        <v>6.366620205925988E-2</v>
+        <v>6.3E-2</v>
       </c>
       <c r="E20" s="1">
         <v>4.6355829324220998E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -808,13 +822,13 @@
         <v>10</v>
       </c>
       <c r="D21" s="1">
-        <v>6.4598520725802189E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="E21" s="1">
         <v>4.7996594476666821E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -825,13 +839,13 @@
         <v>7</v>
       </c>
       <c r="D22" s="1">
-        <v>5.3358345057579082E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="E22" s="1">
         <v>3.0222500130269388E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -842,13 +856,13 @@
         <v>8</v>
       </c>
       <c r="D23" s="1">
-        <v>6.7578874833882918E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="E23" s="1">
         <v>3.4847664517399179E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -859,13 +873,13 @@
         <v>9</v>
       </c>
       <c r="D24" s="1">
-        <v>7.6360536587554373E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="E24" s="1">
         <v>4.8005742743057127E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -876,7 +890,7 @@
         <v>10</v>
       </c>
       <c r="D25" s="1">
-        <v>7.7267818574514036E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="E25" s="1">
         <v>5.2537796976241953E-2</v>

</xml_diff>